<commit_message>
Updating with iperf3 generated at 0.1 seconds
Signed-off-by: Ashish K <akashina@eng.ucsd.edu>
</commit_message>
<xml_diff>
--- a/PriorityExperiments.xlsx
+++ b/PriorityExperiments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak7\OneDrive - UC San Diego\Illinois Urbana Champaign\Repositories\qos_synthesis\priority_validation_expts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak7\OneDrive - UC San Diego\Illinois Urbana Champaign\Repositories\qos_synthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="67">
   <si>
     <t>300k packets @ 100us</t>
   </si>
@@ -294,6 +294,78 @@
       <t>: Saturate the link between s1 and s2 such that the next realtime flow takes the longer hop path (but still has 
 lesser e2e delay)</t>
     </r>
+  </si>
+  <si>
+    <t>(412.95)381.76</t>
+  </si>
+  <si>
+    <t>(415.93)401.2</t>
+  </si>
+  <si>
+    <t>(426.3)408.38</t>
+  </si>
+  <si>
+    <t>(428.98)436.65</t>
+  </si>
+  <si>
+    <t>(426.62)439.61</t>
+  </si>
+  <si>
+    <t>(421.91)411.09</t>
+  </si>
+  <si>
+    <t>(412.04)394.29</t>
+  </si>
+  <si>
+    <t>(398.71)394.87</t>
+  </si>
+  <si>
+    <t>(430.94)442.15</t>
+  </si>
+  <si>
+    <t>(417.12)416.06</t>
+  </si>
+  <si>
+    <t>(412.63)395.52</t>
+  </si>
+  <si>
+    <t>(406.6)392.11</t>
+  </si>
+  <si>
+    <t>(437.15)442.24</t>
+  </si>
+  <si>
+    <t>(425.8)417.43</t>
+  </si>
+  <si>
+    <t>(419.68)403.1</t>
+  </si>
+  <si>
+    <t>(415.02)407.49</t>
+  </si>
+  <si>
+    <t>(436.6)441.89</t>
+  </si>
+  <si>
+    <t>(433.25)382.8</t>
+  </si>
+  <si>
+    <t>(433.27)405.87</t>
+  </si>
+  <si>
+    <t>(431.9)414.49</t>
+  </si>
+  <si>
+    <t>(435.41)441.3</t>
+  </si>
+  <si>
+    <t>(423.59)415.21</t>
+  </si>
+  <si>
+    <t>(430.68)412.6</t>
+  </si>
+  <si>
+    <t>(412.875)389.62</t>
   </si>
 </sst>
 </file>
@@ -398,6 +470,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -407,22 +492,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -813,58 +885,58 @@
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="3"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="11"/>
+      <c r="H2" s="18"/>
       <c r="I2" s="3"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="11"/>
+      <c r="L2" s="18"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="11"/>
+      <c r="P2" s="18"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="6"/>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="11"/>
+      <c r="T2" s="18"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1059,248 +1131,248 @@
       <c r="R7" s="8"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
     </row>
     <row r="22" spans="1:20" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1322,7 +1394,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,86 +1406,86 @@
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="11" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="12"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15" t="s">
+      <c r="E3" s="19"/>
+      <c r="F3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="15" t="s">
+      <c r="G3" s="19"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15" t="s">
+      <c r="J3" s="19"/>
+      <c r="K3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15" t="s">
+      <c r="L3" s="19"/>
+      <c r="M3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="13"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1434,7 +1506,7 @@
       <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="14"/>
+      <c r="H4" s="11"/>
       <c r="I4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1453,57 +1525,57 @@
       <c r="N4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="14"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5">
-        <v>382.8</v>
+      <c r="B5" t="s">
+        <v>60</v>
       </c>
       <c r="D5">
         <v>384.2</v>
       </c>
-      <c r="F5">
-        <v>381.76</v>
-      </c>
-      <c r="H5" s="14"/>
-      <c r="I5">
-        <v>405.87</v>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" t="s">
+        <v>61</v>
       </c>
       <c r="K5">
         <v>401.83</v>
       </c>
-      <c r="M5">
-        <v>401.2</v>
-      </c>
-      <c r="O5" s="14"/>
+      <c r="M5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="11"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B6">
-        <v>389.62</v>
-      </c>
-      <c r="D6" s="18">
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="14">
         <v>406.3</v>
       </c>
-      <c r="F6">
-        <v>394.87</v>
-      </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="18">
-        <v>412.6</v>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="K6">
         <v>395.01</v>
       </c>
-      <c r="M6">
-        <v>394.29</v>
-      </c>
-      <c r="O6" s="14"/>
+      <c r="M6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="11"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1515,20 +1587,20 @@
       <c r="D7">
         <v>408.64</v>
       </c>
-      <c r="F7">
-        <v>392.11</v>
-      </c>
-      <c r="H7" s="14"/>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="11"/>
       <c r="I7">
         <v>395.12</v>
       </c>
       <c r="K7">
         <v>398.36</v>
       </c>
-      <c r="M7">
-        <v>395.52</v>
-      </c>
-      <c r="O7" s="14"/>
+      <c r="M7" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="11"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1540,103 +1612,103 @@
       <c r="D8">
         <v>370.46</v>
       </c>
-      <c r="F8" s="18">
-        <v>407.49</v>
-      </c>
-      <c r="H8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="11"/>
       <c r="I8">
         <v>402.66</v>
       </c>
       <c r="K8">
         <v>399.6</v>
       </c>
-      <c r="M8">
-        <v>403.1</v>
-      </c>
-      <c r="O8" s="14"/>
+      <c r="M8" t="s">
+        <v>57</v>
+      </c>
+      <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="11" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="14"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15" t="s">
+      <c r="E12" s="19"/>
+      <c r="F12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="15" t="s">
+      <c r="G12" s="19"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15" t="s">
+      <c r="J12" s="19"/>
+      <c r="K12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15" t="s">
+      <c r="L12" s="19"/>
+      <c r="M12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="15"/>
-      <c r="O12" s="14"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="11"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -1657,7 +1729,7 @@
       <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="14"/>
+      <c r="H13" s="11"/>
       <c r="I13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1676,57 +1748,57 @@
       <c r="N13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="14"/>
+      <c r="O13" s="11"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B14">
-        <v>414.49</v>
+      <c r="B14" t="s">
+        <v>62</v>
       </c>
       <c r="D14">
         <v>416.14</v>
       </c>
-      <c r="F14">
-        <v>408.38</v>
-      </c>
-      <c r="H14" s="14"/>
-      <c r="I14">
-        <v>441.89</v>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" t="s">
+        <v>59</v>
       </c>
       <c r="K14">
         <v>440.53</v>
       </c>
-      <c r="M14">
-        <v>436.65</v>
-      </c>
-      <c r="O14" s="14"/>
+      <c r="M14" t="s">
+        <v>46</v>
+      </c>
+      <c r="O14" s="11"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B15">
-        <v>415.21</v>
+      <c r="B15" t="s">
+        <v>64</v>
       </c>
       <c r="D15">
         <v>412.3</v>
       </c>
-      <c r="F15">
-        <v>411.09</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15">
-        <v>441.3</v>
+      <c r="F15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" t="s">
+        <v>63</v>
       </c>
       <c r="K15">
         <v>439.81</v>
       </c>
-      <c r="M15">
-        <v>439.61</v>
-      </c>
-      <c r="O15" s="14"/>
+      <c r="M15" t="s">
+        <v>47</v>
+      </c>
+      <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1738,20 +1810,20 @@
       <c r="D16">
         <v>410.49</v>
       </c>
-      <c r="F16">
-        <v>416.06</v>
-      </c>
-      <c r="H16" s="14"/>
+      <c r="F16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="11"/>
       <c r="I16">
         <v>445.3</v>
       </c>
       <c r="K16">
         <v>446.03</v>
       </c>
-      <c r="M16">
-        <v>442.15</v>
-      </c>
-      <c r="O16" s="14"/>
+      <c r="M16" t="s">
+        <v>51</v>
+      </c>
+      <c r="O16" s="11"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1763,66 +1835,66 @@
       <c r="D17">
         <v>408.15</v>
       </c>
-      <c r="F17">
-        <v>417.43</v>
-      </c>
-      <c r="H17" s="14"/>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="11"/>
       <c r="I17">
         <v>441.48</v>
       </c>
       <c r="K17">
         <v>444.10399999999998</v>
       </c>
-      <c r="M17">
-        <v>442.24</v>
-      </c>
-      <c r="O17" s="14"/>
+      <c r="M17" t="s">
+        <v>55</v>
+      </c>
+      <c r="O17" s="11"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="10" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="17" t="s">
         <v>41</v>
       </c>
       <c r="J20" s="20"/>
@@ -1830,30 +1902,30 @@
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
       <c r="N20" s="20"/>
-      <c r="O20" s="14"/>
+      <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15" t="s">
+      <c r="C21" s="19"/>
+      <c r="D21" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15" t="s">
+      <c r="E21" s="19"/>
+      <c r="F21" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="14"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="11"/>
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
       <c r="N21" s="20"/>
-      <c r="O21" s="14"/>
+      <c r="O21" s="11"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
@@ -1874,149 +1946,147 @@
       <c r="G22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="14"/>
+      <c r="H22" s="11"/>
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
       <c r="N22" s="20"/>
-      <c r="O22" s="14"/>
+      <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="14"/>
+      <c r="B23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="11"/>
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
       <c r="N23" s="20"/>
-      <c r="O23" s="14"/>
+      <c r="O23" s="11"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="14"/>
+      <c r="B24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="11"/>
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
       <c r="N24" s="20"/>
-      <c r="O24" s="14"/>
+      <c r="O24" s="11"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="14"/>
+      <c r="B25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="11"/>
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
       <c r="N25" s="20"/>
-      <c r="O25" s="14"/>
+      <c r="O25" s="11"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" s="14"/>
+      <c r="B26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="11"/>
       <c r="I26" s="20"/>
       <c r="J26" s="20"/>
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
-      <c r="O26" s="14"/>
+      <c r="O26" s="11"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="22">
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I20:N26"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="A1:O1"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="I11:N11"/>
@@ -2027,11 +2097,13 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I20:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2042,14 +2114,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="R29:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29:AC37"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="29" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R29" s="10" t="s">
+      <c r="R29" s="17" t="s">
         <v>42</v>
       </c>
       <c r="S29" s="20"/>

</xml_diff>

<commit_message>
More data on iperf3 at 100ms Signed-off-by: Ashish K <akashina@eng.ucsd.edu>
</commit_message>
<xml_diff>
--- a/PriorityExperiments.xlsx
+++ b/PriorityExperiments.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="72">
   <si>
     <t>300k packets @ 100us</t>
   </si>
@@ -366,6 +366,21 @@
   </si>
   <si>
     <t>(412.875)389.62</t>
+  </si>
+  <si>
+    <t>(426.12)377.85</t>
+  </si>
+  <si>
+    <t>(415.76)395.12</t>
+  </si>
+  <si>
+    <t>(425.69)414.55</t>
+  </si>
+  <si>
+    <t>(437.86)445.3</t>
+  </si>
+  <si>
+    <t>( ) -- iperf3 background at 100 ms</t>
   </si>
 </sst>
 </file>
@@ -1391,16 +1406,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
@@ -1581,8 +1596,8 @@
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B7">
-        <v>377.85</v>
+      <c r="B7" t="s">
+        <v>67</v>
       </c>
       <c r="D7">
         <v>408.64</v>
@@ -1591,8 +1606,8 @@
         <v>54</v>
       </c>
       <c r="H7" s="11"/>
-      <c r="I7">
-        <v>395.12</v>
+      <c r="I7" t="s">
+        <v>68</v>
       </c>
       <c r="K7">
         <v>398.36</v>
@@ -1804,8 +1819,8 @@
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16">
-        <v>414.55</v>
+      <c r="B16" t="s">
+        <v>69</v>
       </c>
       <c r="D16">
         <v>410.49</v>
@@ -1814,8 +1829,8 @@
         <v>52</v>
       </c>
       <c r="H16" s="11"/>
-      <c r="I16">
-        <v>445.3</v>
+      <c r="I16" t="s">
+        <v>70</v>
       </c>
       <c r="K16">
         <v>446.03</v>
@@ -2079,31 +2094,36 @@
       <c r="N26" s="20"/>
       <c r="O26" s="11"/>
     </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="22">
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I20:N26"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="I11:N11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="M3:N3"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="I11:N11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="I12:J12"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I20:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated all the 1link measurements and added the raw data in ingress_filtering_expts/with iperf at 100ms/
Signed-off-by: Ashish K <akashina@eng.ucsd.edu>
</commit_message>
<xml_diff>
--- a/PriorityExperiments.xlsx
+++ b/PriorityExperiments.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="77">
   <si>
     <t>300k packets @ 100us</t>
   </si>
@@ -381,6 +381,21 @@
   </si>
   <si>
     <t>( ) -- iperf3 background at 100 ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>(409.48)386.48</t>
+  </si>
+  <si>
+    <t>(413.53)402.66</t>
+  </si>
+  <si>
+    <t>(414.36)414.48</t>
+  </si>
+  <si>
+    <t>(430.54)441.48</t>
   </si>
 </sst>
 </file>
@@ -1406,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,8 +1636,8 @@
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8">
-        <v>386.48</v>
+      <c r="B8" t="s">
+        <v>73</v>
       </c>
       <c r="D8">
         <v>370.46</v>
@@ -1631,8 +1646,8 @@
         <v>58</v>
       </c>
       <c r="H8" s="11"/>
-      <c r="I8">
-        <v>402.66</v>
+      <c r="I8" t="s">
+        <v>74</v>
       </c>
       <c r="K8">
         <v>399.6</v>
@@ -1844,8 +1859,8 @@
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B17">
-        <v>414.48</v>
+      <c r="B17" t="s">
+        <v>75</v>
       </c>
       <c r="D17">
         <v>408.15</v>
@@ -1854,8 +1869,8 @@
         <v>56</v>
       </c>
       <c r="H17" s="11"/>
-      <c r="I17">
-        <v>441.48</v>
+      <c r="I17" t="s">
+        <v>76</v>
       </c>
       <c r="K17">
         <v>444.10399999999998</v>
@@ -2097,6 +2112,11 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the data with custom traffic generator and sleep Signed-off-by: Ashish K <akashina@eng.ucsd.edu>
</commit_message>
<xml_diff>
--- a/PriorityExperiments.xlsx
+++ b/PriorityExperiments.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="505" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Priority Works!" sheetId="1" r:id="rId1"/>
     <sheet name="High Priority Variation Debug" sheetId="2" r:id="rId2"/>
-    <sheet name="Better than Djikstra" sheetId="3" r:id="rId3"/>
+    <sheet name="Custome BG Traffic Gen + Optzns" sheetId="4" r:id="rId3"/>
+    <sheet name="Better than Djikstra" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="94">
   <si>
     <t>300k packets @ 100us</t>
   </si>
@@ -397,12 +398,171 @@
   <si>
     <t>(430.54)441.48</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Experiment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The background traffic is suspected to have varying amount of interference since it could be generated at a coarser granularity.  So we generate iperf at 100ms interval(max resolution supported by iperf3)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Observation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> We see this is indeed the case, since the numbers get closer to one another as we increase the rt traffic from 300k@100us --&gt; 60k@10000us.
+Note that a few anomalies do come in when we try sending packets at 100us and also have interference at 100ms.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Optimization</t>
+  </si>
+  <si>
+    <t>1. Sleep time accuracy</t>
+  </si>
+  <si>
+    <t>Packet Period(us)</t>
+  </si>
+  <si>
+    <t>Time in sendto(us)</t>
+  </si>
+  <si>
+    <t>Time actually sleeping</t>
+  </si>
+  <si>
+    <t>1000M</t>
+  </si>
+  <si>
+    <t>8K</t>
+  </si>
+  <si>
+    <t>Rates(bps)</t>
+  </si>
+  <si>
+    <t>Packet Size(bits)</t>
+  </si>
+  <si>
+    <t>Remaining time actually in sleep()</t>
+  </si>
+  <si>
+    <t>Time between packets(us)</t>
+  </si>
+  <si>
+    <t>1hour</t>
+  </si>
+  <si>
+    <t>30 mins</t>
+  </si>
+  <si>
+    <t>No Sleep</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4us</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Experiment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: We use our custom client-server traffic generator to generate as fast traffic as possible.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Idea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Observation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Traffic generation doesn't seem high bandwidth enough for us to use since the low priority flow is able to use the slack in the network bandwidth to get through.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,8 +592,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,6 +646,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -478,7 +666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -513,6 +701,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -523,11 +723,47 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,58 +1151,58 @@
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="18"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="3"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="18"/>
+      <c r="H2" s="22"/>
       <c r="I2" s="3"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="18"/>
+      <c r="L2" s="22"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="18"/>
+      <c r="P2" s="22"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="6"/>
-      <c r="S2" s="18" t="s">
+      <c r="S2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="18"/>
+      <c r="T2" s="22"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1161,248 +1397,248 @@
       <c r="R7" s="8"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="17"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
     </row>
     <row r="22" spans="1:20" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1421,10 +1657,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,72 +1682,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19" t="s">
+      <c r="J3" s="25"/>
+      <c r="K3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19" t="s">
+      <c r="L3" s="25"/>
+      <c r="M3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="19"/>
+      <c r="N3" s="25"/>
       <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1692,52 +1928,52 @@
       <c r="O10" s="12"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
       <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19" t="s">
+      <c r="C12" s="25"/>
+      <c r="D12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19" t="s">
+      <c r="E12" s="25"/>
+      <c r="F12" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="19"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19" t="s">
+      <c r="J12" s="25"/>
+      <c r="K12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19" t="s">
+      <c r="L12" s="25"/>
+      <c r="M12" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="19"/>
+      <c r="N12" s="25"/>
       <c r="O12" s="11"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1915,46 +2151,46 @@
       <c r="O19" s="12"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
       <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19" t="s">
+      <c r="C21" s="25"/>
+      <c r="D21" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19" t="s">
+      <c r="E21" s="25"/>
+      <c r="F21" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
       <c r="O21" s="11"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1977,12 +2213,12 @@
         <v>10</v>
       </c>
       <c r="H22" s="11"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
       <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2008,12 +2244,12 @@
         <v>40</v>
       </c>
       <c r="H23" s="11"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
       <c r="O23" s="11"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2039,12 +2275,12 @@
         <v>40</v>
       </c>
       <c r="H24" s="11"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
       <c r="O24" s="11"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2070,12 +2306,12 @@
         <v>40</v>
       </c>
       <c r="H25" s="11"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
       <c r="O25" s="11"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2101,32 +2337,101 @@
         <v>40</v>
       </c>
       <c r="H26" s="11"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
       <c r="O26" s="11"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I28" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>71</v>
       </c>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>72</v>
       </c>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+    </row>
+    <row r="33" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+    </row>
+    <row r="34" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+    </row>
+    <row r="35" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="24"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="22">
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
+  <mergeCells count="23">
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="I20:N26"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I28:N35"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I2:N2"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="I11:N11"/>
     <mergeCell ref="B12:C12"/>
@@ -2135,15 +2440,9 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="M12:N12"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2151,6 +2450,854 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="17">
+        <v>100</v>
+      </c>
+      <c r="C3" s="17">
+        <v>7</v>
+      </c>
+      <c r="D3" s="17">
+        <f>B3-C3</f>
+        <v>93</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="17">
+        <f>(8000/1000000000)*1000000</f>
+        <v>8</v>
+      </c>
+      <c r="I3" s="17">
+        <v>1</v>
+      </c>
+      <c r="J3" s="17">
+        <f>3600/0.000008</f>
+        <v>450000000</v>
+      </c>
+      <c r="K3" s="19">
+        <f>J3/2</f>
+        <v>225000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="17">
+        <v>500</v>
+      </c>
+      <c r="C4" s="17">
+        <v>18</v>
+      </c>
+      <c r="D4" s="17">
+        <f t="shared" ref="D4:D6" si="0">B4-C4</f>
+        <v>482</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="17">
+        <f>(8000/750000000)*1000000</f>
+        <v>10.666666666666668</v>
+      </c>
+      <c r="I4" s="17">
+        <v>4</v>
+      </c>
+      <c r="J4" s="17">
+        <f>3600/0.000011</f>
+        <v>327272727.27272731</v>
+      </c>
+      <c r="K4" s="19">
+        <f>J4/2</f>
+        <v>163636363.63636366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="17">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="17">
+        <v>39</v>
+      </c>
+      <c r="D5" s="17">
+        <f t="shared" si="0"/>
+        <v>961</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="17">
+        <f>(8000/500000000)*1000000</f>
+        <v>16</v>
+      </c>
+      <c r="I5" s="17">
+        <v>9</v>
+      </c>
+      <c r="J5" s="17">
+        <f>3600/0.000016</f>
+        <v>225000000</v>
+      </c>
+      <c r="K5" s="19">
+        <f>J5/2</f>
+        <v>112500000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17">
+        <v>10000</v>
+      </c>
+      <c r="C6" s="17">
+        <v>43</v>
+      </c>
+      <c r="D6" s="17">
+        <f t="shared" si="0"/>
+        <v>9957</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="17">
+        <f>(8000/250000000)*1000000</f>
+        <v>32</v>
+      </c>
+      <c r="I6" s="17">
+        <v>25</v>
+      </c>
+      <c r="J6" s="17">
+        <f>3600/0.000032</f>
+        <v>112500000</v>
+      </c>
+      <c r="K6" s="19">
+        <f>J6/2</f>
+        <v>56250000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="19">
+        <f>8000/0.01</f>
+        <v>800000</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="17">
+        <v>100</v>
+      </c>
+      <c r="I7" s="17">
+        <v>93</v>
+      </c>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="30"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="33"/>
+      <c r="I11" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" s="27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="34">
+        <v>374.85</v>
+      </c>
+      <c r="C12" s="34">
+        <v>415.34</v>
+      </c>
+      <c r="D12" s="34">
+        <v>366.98</v>
+      </c>
+      <c r="E12" s="34">
+        <v>398.13</v>
+      </c>
+      <c r="F12" s="35">
+        <v>387.3</v>
+      </c>
+      <c r="G12" s="35">
+        <v>315.35000000000002</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34">
+        <v>384.01</v>
+      </c>
+      <c r="J12" s="34">
+        <v>407.92</v>
+      </c>
+      <c r="K12" s="34">
+        <v>386.06</v>
+      </c>
+      <c r="L12" s="34">
+        <v>406.31</v>
+      </c>
+      <c r="M12" s="34">
+        <v>383.38</v>
+      </c>
+      <c r="N12" s="34">
+        <v>406.07</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="34">
+        <v>381.51</v>
+      </c>
+      <c r="C13" s="34">
+        <v>421.74</v>
+      </c>
+      <c r="D13" s="35">
+        <v>344.71</v>
+      </c>
+      <c r="E13" s="34">
+        <v>399.6</v>
+      </c>
+      <c r="F13" s="34">
+        <v>369.4</v>
+      </c>
+      <c r="G13" s="34">
+        <v>400.24</v>
+      </c>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34">
+        <v>388.87</v>
+      </c>
+      <c r="J13" s="36">
+        <v>409.9</v>
+      </c>
+      <c r="K13" s="34">
+        <v>392.51</v>
+      </c>
+      <c r="L13" s="34">
+        <v>413.47</v>
+      </c>
+      <c r="M13" s="34">
+        <v>379.55</v>
+      </c>
+      <c r="N13" s="34">
+        <v>395.22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="30"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" s="30"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="33"/>
+      <c r="I18" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="34">
+        <v>399.19</v>
+      </c>
+      <c r="C19" s="34">
+        <v>419.46</v>
+      </c>
+      <c r="D19" s="34">
+        <v>398.55</v>
+      </c>
+      <c r="E19" s="34">
+        <v>417.53</v>
+      </c>
+      <c r="F19" s="34">
+        <v>406.5</v>
+      </c>
+      <c r="G19" s="34">
+        <v>419.33</v>
+      </c>
+      <c r="H19" s="33"/>
+      <c r="I19" s="34">
+        <v>410.13</v>
+      </c>
+      <c r="J19" s="34">
+        <v>432.42</v>
+      </c>
+      <c r="K19" s="34">
+        <v>409.44</v>
+      </c>
+      <c r="L19" s="34">
+        <v>433.99</v>
+      </c>
+      <c r="M19" s="34">
+        <v>417.48</v>
+      </c>
+      <c r="N19" s="34">
+        <v>432.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="34">
+        <v>407.6</v>
+      </c>
+      <c r="C20" s="34">
+        <v>425.83</v>
+      </c>
+      <c r="D20" s="34">
+        <v>403.92</v>
+      </c>
+      <c r="E20" s="34">
+        <v>417.74</v>
+      </c>
+      <c r="F20" s="34">
+        <v>401.51</v>
+      </c>
+      <c r="G20" s="34">
+        <v>416.84</v>
+      </c>
+      <c r="H20" s="33"/>
+      <c r="I20" s="34">
+        <v>420.73</v>
+      </c>
+      <c r="J20" s="34">
+        <v>434.88</v>
+      </c>
+      <c r="K20" s="34">
+        <v>417.42</v>
+      </c>
+      <c r="L20" s="34">
+        <v>436.56</v>
+      </c>
+      <c r="M20" s="34">
+        <v>408.77</v>
+      </c>
+      <c r="N20" s="34">
+        <v>431.37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="B23" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="30"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
+      <c r="B25" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="33"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="39"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="33"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="33"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="39"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="33"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="H29" s="33"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="I16:N16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="I23:N29"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="R29:AC37"/>
   <sheetViews>
@@ -2161,132 +3308,132 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="29" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R29" s="17" t="s">
+      <c r="R29" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="S29" s="20"/>
-      <c r="T29" s="20"/>
-      <c r="U29" s="20"/>
-      <c r="V29" s="20"/>
-      <c r="W29" s="20"/>
-      <c r="X29" s="20"/>
-      <c r="Y29" s="20"/>
-      <c r="Z29" s="20"/>
-      <c r="AA29" s="20"/>
-      <c r="AB29" s="20"/>
-      <c r="AC29" s="20"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+      <c r="Y29" s="26"/>
+      <c r="Z29" s="26"/>
+      <c r="AA29" s="26"/>
+      <c r="AB29" s="26"/>
+      <c r="AC29" s="26"/>
     </row>
     <row r="30" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R30" s="20"/>
-      <c r="S30" s="20"/>
-      <c r="T30" s="20"/>
-      <c r="U30" s="20"/>
-      <c r="V30" s="20"/>
-      <c r="W30" s="20"/>
-      <c r="X30" s="20"/>
-      <c r="Y30" s="20"/>
-      <c r="Z30" s="20"/>
-      <c r="AA30" s="20"/>
-      <c r="AB30" s="20"/>
-      <c r="AC30" s="20"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="26"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="26"/>
+      <c r="X30" s="26"/>
+      <c r="Y30" s="26"/>
+      <c r="Z30" s="26"/>
+      <c r="AA30" s="26"/>
+      <c r="AB30" s="26"/>
+      <c r="AC30" s="26"/>
     </row>
     <row r="31" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R31" s="20"/>
-      <c r="S31" s="20"/>
-      <c r="T31" s="20"/>
-      <c r="U31" s="20"/>
-      <c r="V31" s="20"/>
-      <c r="W31" s="20"/>
-      <c r="X31" s="20"/>
-      <c r="Y31" s="20"/>
-      <c r="Z31" s="20"/>
-      <c r="AA31" s="20"/>
-      <c r="AB31" s="20"/>
-      <c r="AC31" s="20"/>
+      <c r="R31" s="26"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="26"/>
+      <c r="U31" s="26"/>
+      <c r="V31" s="26"/>
+      <c r="W31" s="26"/>
+      <c r="X31" s="26"/>
+      <c r="Y31" s="26"/>
+      <c r="Z31" s="26"/>
+      <c r="AA31" s="26"/>
+      <c r="AB31" s="26"/>
+      <c r="AC31" s="26"/>
     </row>
     <row r="32" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R32" s="20"/>
-      <c r="S32" s="20"/>
-      <c r="T32" s="20"/>
-      <c r="U32" s="20"/>
-      <c r="V32" s="20"/>
-      <c r="W32" s="20"/>
-      <c r="X32" s="20"/>
-      <c r="Y32" s="20"/>
-      <c r="Z32" s="20"/>
-      <c r="AA32" s="20"/>
-      <c r="AB32" s="20"/>
-      <c r="AC32" s="20"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="26"/>
+      <c r="V32" s="26"/>
+      <c r="W32" s="26"/>
+      <c r="X32" s="26"/>
+      <c r="Y32" s="26"/>
+      <c r="Z32" s="26"/>
+      <c r="AA32" s="26"/>
+      <c r="AB32" s="26"/>
+      <c r="AC32" s="26"/>
     </row>
     <row r="33" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R33" s="20"/>
-      <c r="S33" s="20"/>
-      <c r="T33" s="20"/>
-      <c r="U33" s="20"/>
-      <c r="V33" s="20"/>
-      <c r="W33" s="20"/>
-      <c r="X33" s="20"/>
-      <c r="Y33" s="20"/>
-      <c r="Z33" s="20"/>
-      <c r="AA33" s="20"/>
-      <c r="AB33" s="20"/>
-      <c r="AC33" s="20"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="26"/>
+      <c r="X33" s="26"/>
+      <c r="Y33" s="26"/>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="26"/>
+      <c r="AB33" s="26"/>
+      <c r="AC33" s="26"/>
     </row>
     <row r="34" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R34" s="20"/>
-      <c r="S34" s="20"/>
-      <c r="T34" s="20"/>
-      <c r="U34" s="20"/>
-      <c r="V34" s="20"/>
-      <c r="W34" s="20"/>
-      <c r="X34" s="20"/>
-      <c r="Y34" s="20"/>
-      <c r="Z34" s="20"/>
-      <c r="AA34" s="20"/>
-      <c r="AB34" s="20"/>
-      <c r="AC34" s="20"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="26"/>
+      <c r="T34" s="26"/>
+      <c r="U34" s="26"/>
+      <c r="V34" s="26"/>
+      <c r="W34" s="26"/>
+      <c r="X34" s="26"/>
+      <c r="Y34" s="26"/>
+      <c r="Z34" s="26"/>
+      <c r="AA34" s="26"/>
+      <c r="AB34" s="26"/>
+      <c r="AC34" s="26"/>
     </row>
     <row r="35" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R35" s="20"/>
-      <c r="S35" s="20"/>
-      <c r="T35" s="20"/>
-      <c r="U35" s="20"/>
-      <c r="V35" s="20"/>
-      <c r="W35" s="20"/>
-      <c r="X35" s="20"/>
-      <c r="Y35" s="20"/>
-      <c r="Z35" s="20"/>
-      <c r="AA35" s="20"/>
-      <c r="AB35" s="20"/>
-      <c r="AC35" s="20"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="26"/>
+      <c r="T35" s="26"/>
+      <c r="U35" s="26"/>
+      <c r="V35" s="26"/>
+      <c r="W35" s="26"/>
+      <c r="X35" s="26"/>
+      <c r="Y35" s="26"/>
+      <c r="Z35" s="26"/>
+      <c r="AA35" s="26"/>
+      <c r="AB35" s="26"/>
+      <c r="AC35" s="26"/>
     </row>
     <row r="36" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R36" s="20"/>
-      <c r="S36" s="20"/>
-      <c r="T36" s="20"/>
-      <c r="U36" s="20"/>
-      <c r="V36" s="20"/>
-      <c r="W36" s="20"/>
-      <c r="X36" s="20"/>
-      <c r="Y36" s="20"/>
-      <c r="Z36" s="20"/>
-      <c r="AA36" s="20"/>
-      <c r="AB36" s="20"/>
-      <c r="AC36" s="20"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="26"/>
+      <c r="T36" s="26"/>
+      <c r="U36" s="26"/>
+      <c r="V36" s="26"/>
+      <c r="W36" s="26"/>
+      <c r="X36" s="26"/>
+      <c r="Y36" s="26"/>
+      <c r="Z36" s="26"/>
+      <c r="AA36" s="26"/>
+      <c r="AB36" s="26"/>
+      <c r="AC36" s="26"/>
     </row>
     <row r="37" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R37" s="20"/>
-      <c r="S37" s="20"/>
-      <c r="T37" s="20"/>
-      <c r="U37" s="20"/>
-      <c r="V37" s="20"/>
-      <c r="W37" s="20"/>
-      <c r="X37" s="20"/>
-      <c r="Y37" s="20"/>
-      <c r="Z37" s="20"/>
-      <c r="AA37" s="20"/>
-      <c r="AB37" s="20"/>
-      <c r="AC37" s="20"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="26"/>
+      <c r="V37" s="26"/>
+      <c r="W37" s="26"/>
+      <c r="X37" s="26"/>
+      <c r="Y37" s="26"/>
+      <c r="Z37" s="26"/>
+      <c r="AA37" s="26"/>
+      <c r="AB37" s="26"/>
+      <c r="AC37" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Signed-off-by: Ashish K <akashina@eng.ucsd.edu>
</commit_message>
<xml_diff>
--- a/PriorityExperiments.xlsx
+++ b/PriorityExperiments.xlsx
@@ -14,8 +14,9 @@
   <sheets>
     <sheet name="Priority Works!" sheetId="1" r:id="rId1"/>
     <sheet name="High Priority Variation Debug" sheetId="2" r:id="rId2"/>
-    <sheet name="Custome BG Traffic Gen + Optzns" sheetId="4" r:id="rId3"/>
-    <sheet name="Better than Djikstra" sheetId="3" r:id="rId4"/>
+    <sheet name="iperf at 0.1" sheetId="5" r:id="rId3"/>
+    <sheet name="Custome BG Traffic Gen + Optzns" sheetId="4" r:id="rId4"/>
+    <sheet name="Better than Djikstra" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="82">
   <si>
     <t>300k packets @ 100us</t>
   </si>
@@ -297,106 +298,7 @@
     </r>
   </si>
   <si>
-    <t>(412.95)381.76</t>
-  </si>
-  <si>
-    <t>(415.93)401.2</t>
-  </si>
-  <si>
-    <t>(426.3)408.38</t>
-  </si>
-  <si>
-    <t>(428.98)436.65</t>
-  </si>
-  <si>
-    <t>(426.62)439.61</t>
-  </si>
-  <si>
-    <t>(421.91)411.09</t>
-  </si>
-  <si>
-    <t>(412.04)394.29</t>
-  </si>
-  <si>
-    <t>(398.71)394.87</t>
-  </si>
-  <si>
-    <t>(430.94)442.15</t>
-  </si>
-  <si>
-    <t>(417.12)416.06</t>
-  </si>
-  <si>
-    <t>(412.63)395.52</t>
-  </si>
-  <si>
-    <t>(406.6)392.11</t>
-  </si>
-  <si>
-    <t>(437.15)442.24</t>
-  </si>
-  <si>
-    <t>(425.8)417.43</t>
-  </si>
-  <si>
-    <t>(419.68)403.1</t>
-  </si>
-  <si>
-    <t>(415.02)407.49</t>
-  </si>
-  <si>
-    <t>(436.6)441.89</t>
-  </si>
-  <si>
-    <t>(433.25)382.8</t>
-  </si>
-  <si>
-    <t>(433.27)405.87</t>
-  </si>
-  <si>
-    <t>(431.9)414.49</t>
-  </si>
-  <si>
-    <t>(435.41)441.3</t>
-  </si>
-  <si>
-    <t>(423.59)415.21</t>
-  </si>
-  <si>
-    <t>(430.68)412.6</t>
-  </si>
-  <si>
-    <t>(412.875)389.62</t>
-  </si>
-  <si>
-    <t>(426.12)377.85</t>
-  </si>
-  <si>
-    <t>(415.76)395.12</t>
-  </si>
-  <si>
-    <t>(425.69)414.55</t>
-  </si>
-  <si>
-    <t>(437.86)445.3</t>
-  </si>
-  <si>
-    <t>( ) -- iperf3 background at 100 ms</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>(409.48)386.48</t>
-  </si>
-  <si>
-    <t>(413.53)402.66</t>
-  </si>
-  <si>
-    <t>(414.36)414.48</t>
-  </si>
-  <si>
-    <t>(430.54)441.48</t>
   </si>
   <si>
     <r>
@@ -556,6 +458,113 @@
       </rPr>
       <t>: Traffic generation doesn't seem high bandwidth enough for us to use since the low priority flow is able to use the slack in the network bandwidth to get through.</t>
     </r>
+  </si>
+  <si>
+    <t>300k packets@100us</t>
+  </si>
+  <si>
+    <t>300k packets@500us</t>
+  </si>
+  <si>
+    <t>300k packets@1000us</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Experiment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The background traffic is suspected to have varying amount of interference since it could be generated at a coarser granularity.  So we generate iperf at 100ms interval(max resolution supported by iperf3) -- data in next sheet
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Observation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> We see this is indeed the case, since the numbers get closer to one another as we increase the rt traffic from 300k@100us --&gt; 60k@10000us.
+Note that a few anomalies do come in when we try sending packets at 100us and also have interference at 100ms.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>1.6 s</t>
+  </si>
+  <si>
+    <t>1.46 s</t>
+  </si>
+  <si>
+    <t>11.51 s</t>
+  </si>
+  <si>
+    <t>10.88 s</t>
+  </si>
+  <si>
+    <t>882 ms</t>
+  </si>
+  <si>
+    <t>836 ms</t>
+  </si>
+  <si>
+    <t>342 ms</t>
+  </si>
+  <si>
+    <t>1.53 s</t>
+  </si>
+  <si>
+    <t>1.25s</t>
+  </si>
+  <si>
+    <t>1.05 s</t>
+  </si>
+  <si>
+    <t>984 ms</t>
+  </si>
+  <si>
+    <t>699.8 ms</t>
+  </si>
+  <si>
+    <t>714.71 ms</t>
+  </si>
+  <si>
+    <t>1.19 ms</t>
+  </si>
+  <si>
+    <t>2.49 ms</t>
+  </si>
+  <si>
+    <t>8.60 ms</t>
+  </si>
+  <si>
+    <t>318 ms</t>
   </si>
 </sst>
 </file>
@@ -666,7 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -713,31 +722,13 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -757,13 +748,43 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1151,58 +1172,58 @@
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="22"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="3"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="35"/>
       <c r="I2" s="3"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="22"/>
+      <c r="L2" s="35"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="22"/>
+      <c r="P2" s="35"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="6"/>
-      <c r="S2" s="22" t="s">
+      <c r="S2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="22"/>
+      <c r="T2" s="35"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1397,248 +1418,248 @@
       <c r="R7" s="8"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="34"/>
+      <c r="T17" s="34"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="34"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="34"/>
+      <c r="T19" s="34"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="34"/>
+      <c r="T20" s="34"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="34"/>
     </row>
     <row r="22" spans="1:20" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="34"/>
+      <c r="T22" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1660,7 +1681,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N26"/>
+      <selection activeCell="I28" sqref="I28:N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,72 +1703,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="36"/>
+      <c r="F3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="36"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25" t="s">
+      <c r="J3" s="36"/>
+      <c r="K3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25" t="s">
+      <c r="L3" s="36"/>
+      <c r="M3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="25"/>
+      <c r="N3" s="36"/>
       <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1797,24 +1818,24 @@
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
-        <v>60</v>
+      <c r="B5">
+        <v>382.8</v>
       </c>
       <c r="D5">
         <v>384.2</v>
       </c>
-      <c r="F5" t="s">
-        <v>43</v>
+      <c r="F5">
+        <v>381.76</v>
       </c>
       <c r="H5" s="11"/>
-      <c r="I5" t="s">
-        <v>61</v>
+      <c r="I5">
+        <v>405.87</v>
       </c>
       <c r="K5">
         <v>401.83</v>
       </c>
-      <c r="M5" t="s">
-        <v>44</v>
+      <c r="M5">
+        <v>401.2</v>
       </c>
       <c r="O5" s="11"/>
     </row>
@@ -1822,24 +1843,24 @@
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
-        <v>66</v>
+      <c r="B6">
+        <v>389.62</v>
       </c>
       <c r="D6" s="14">
         <v>406.3</v>
       </c>
-      <c r="F6" t="s">
-        <v>50</v>
+      <c r="F6">
+        <v>394.87</v>
       </c>
       <c r="H6" s="11"/>
-      <c r="I6" s="14" t="s">
-        <v>65</v>
+      <c r="I6" s="14">
+        <v>412.6</v>
       </c>
       <c r="K6">
         <v>395.01</v>
       </c>
-      <c r="M6" t="s">
-        <v>49</v>
+      <c r="M6">
+        <v>394.29</v>
       </c>
       <c r="O6" s="11"/>
     </row>
@@ -1847,24 +1868,24 @@
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
-        <v>67</v>
+      <c r="B7">
+        <v>377.85</v>
       </c>
       <c r="D7">
         <v>408.64</v>
       </c>
-      <c r="F7" t="s">
-        <v>54</v>
+      <c r="F7">
+        <v>392.11</v>
       </c>
       <c r="H7" s="11"/>
-      <c r="I7" t="s">
-        <v>68</v>
+      <c r="I7">
+        <v>395.12</v>
       </c>
       <c r="K7">
         <v>398.36</v>
       </c>
-      <c r="M7" t="s">
-        <v>53</v>
+      <c r="M7">
+        <v>395.52</v>
       </c>
       <c r="O7" s="11"/>
     </row>
@@ -1872,24 +1893,24 @@
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s">
-        <v>73</v>
+      <c r="B8">
+        <v>386.48</v>
       </c>
       <c r="D8">
         <v>370.46</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>58</v>
+      <c r="F8" s="14">
+        <v>407.49</v>
       </c>
       <c r="H8" s="11"/>
-      <c r="I8" t="s">
-        <v>74</v>
+      <c r="I8">
+        <v>402.66</v>
       </c>
       <c r="K8">
         <v>399.6</v>
       </c>
-      <c r="M8" t="s">
-        <v>57</v>
+      <c r="M8">
+        <v>403.1</v>
       </c>
       <c r="O8" s="11"/>
     </row>
@@ -1928,52 +1949,52 @@
       <c r="O10" s="12"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
       <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25" t="s">
+      <c r="C12" s="36"/>
+      <c r="D12" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25" t="s">
+      <c r="E12" s="36"/>
+      <c r="F12" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="25"/>
+      <c r="G12" s="36"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25" t="s">
+      <c r="J12" s="36"/>
+      <c r="K12" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25" t="s">
+      <c r="L12" s="36"/>
+      <c r="M12" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="25"/>
+      <c r="N12" s="36"/>
       <c r="O12" s="11"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2020,24 +2041,24 @@
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
-        <v>62</v>
+      <c r="B14">
+        <v>414.49</v>
       </c>
       <c r="D14">
         <v>416.14</v>
       </c>
-      <c r="F14" t="s">
-        <v>45</v>
+      <c r="F14">
+        <v>408.38</v>
       </c>
       <c r="H14" s="11"/>
-      <c r="I14" t="s">
-        <v>59</v>
+      <c r="I14">
+        <v>441.89</v>
       </c>
       <c r="K14">
         <v>440.53</v>
       </c>
-      <c r="M14" t="s">
-        <v>46</v>
+      <c r="M14">
+        <v>436.65</v>
       </c>
       <c r="O14" s="11"/>
     </row>
@@ -2045,24 +2066,24 @@
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
-        <v>64</v>
+      <c r="B15">
+        <v>415.21</v>
       </c>
       <c r="D15">
         <v>412.3</v>
       </c>
-      <c r="F15" t="s">
-        <v>48</v>
+      <c r="F15">
+        <v>411.09</v>
       </c>
       <c r="H15" s="11"/>
-      <c r="I15" t="s">
-        <v>63</v>
+      <c r="I15">
+        <v>441.3</v>
       </c>
       <c r="K15">
         <v>439.81</v>
       </c>
-      <c r="M15" t="s">
-        <v>47</v>
+      <c r="M15">
+        <v>439.61</v>
       </c>
       <c r="O15" s="11"/>
     </row>
@@ -2070,24 +2091,24 @@
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
-        <v>69</v>
+      <c r="B16">
+        <v>414.55</v>
       </c>
       <c r="D16">
         <v>410.49</v>
       </c>
-      <c r="F16" t="s">
-        <v>52</v>
+      <c r="F16">
+        <v>416.06</v>
       </c>
       <c r="H16" s="11"/>
-      <c r="I16" t="s">
-        <v>70</v>
+      <c r="I16">
+        <v>445.3</v>
       </c>
       <c r="K16">
         <v>446.03</v>
       </c>
-      <c r="M16" t="s">
-        <v>51</v>
+      <c r="M16">
+        <v>442.15</v>
       </c>
       <c r="O16" s="11"/>
     </row>
@@ -2095,24 +2116,24 @@
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
-        <v>75</v>
+      <c r="B17">
+        <v>414.48</v>
       </c>
       <c r="D17">
         <v>408.15</v>
       </c>
-      <c r="F17" t="s">
-        <v>56</v>
+      <c r="F17">
+        <v>417.43</v>
       </c>
       <c r="H17" s="11"/>
-      <c r="I17" t="s">
-        <v>76</v>
+      <c r="I17">
+        <v>441.48</v>
       </c>
       <c r="K17">
         <v>444.10399999999998</v>
       </c>
-      <c r="M17" t="s">
-        <v>55</v>
+      <c r="M17">
+        <v>442.24</v>
       </c>
       <c r="O17" s="11"/>
     </row>
@@ -2151,46 +2172,46 @@
       <c r="O19" s="12"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="21" t="s">
+      <c r="I20" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
       <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25" t="s">
+      <c r="C21" s="36"/>
+      <c r="D21" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25" t="s">
+      <c r="E21" s="36"/>
+      <c r="F21" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="25"/>
+      <c r="G21" s="36"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
       <c r="O21" s="11"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2213,12 +2234,12 @@
         <v>10</v>
       </c>
       <c r="H22" s="11"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
       <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2244,12 +2265,12 @@
         <v>40</v>
       </c>
       <c r="H23" s="11"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
       <c r="O23" s="11"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2275,12 +2296,12 @@
         <v>40</v>
       </c>
       <c r="H24" s="11"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
       <c r="O24" s="11"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2306,12 +2327,12 @@
         <v>40</v>
       </c>
       <c r="H25" s="11"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
       <c r="O25" s="11"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2337,96 +2358,86 @@
         <v>40</v>
       </c>
       <c r="H26" s="11"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
       <c r="O26" s="11"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I28" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
+      <c r="I28" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>71</v>
-      </c>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>72</v>
-      </c>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+        <v>43</v>
+      </c>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="39"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
     </row>
     <row r="33" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="24"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="39"/>
     </row>
     <row r="34" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="24"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
     </row>
     <row r="35" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="24"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="39"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="23">
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I20:N26"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="I28:N35"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="I3:J3"/>
@@ -2443,6 +2454,13 @@
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I20:N26"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2451,10 +2469,839 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="36"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="36"/>
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="11"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>433.25</v>
+      </c>
+      <c r="F5">
+        <v>412.95</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5">
+        <v>433.27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5">
+        <v>415.93</v>
+      </c>
+      <c r="N5" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" s="11"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <v>412.875</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="F6">
+        <v>398.71</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="14">
+        <v>430.68</v>
+      </c>
+      <c r="J6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6">
+        <v>412.04</v>
+      </c>
+      <c r="N6" t="s">
+        <v>75</v>
+      </c>
+      <c r="O6" s="11"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>426.12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7">
+        <v>406.6</v>
+      </c>
+      <c r="G7">
+        <v>8.92</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7">
+        <v>415.76</v>
+      </c>
+      <c r="J7" t="s">
+        <v>72</v>
+      </c>
+      <c r="M7">
+        <v>412.63</v>
+      </c>
+      <c r="N7" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" s="11"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>409.48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="14">
+        <v>415.02</v>
+      </c>
+      <c r="G8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8">
+        <v>413.53</v>
+      </c>
+      <c r="J8">
+        <v>743.5</v>
+      </c>
+      <c r="M8">
+        <v>419.68</v>
+      </c>
+      <c r="N8" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8" s="11"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="11"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" s="36"/>
+      <c r="O12" s="11"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <v>431.9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14">
+        <v>426.3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14">
+        <v>436.6</v>
+      </c>
+      <c r="J14" s="14">
+        <v>463.96</v>
+      </c>
+      <c r="M14">
+        <v>428.98</v>
+      </c>
+      <c r="N14" s="14">
+        <v>454.17500000000001</v>
+      </c>
+      <c r="O14" s="11"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <v>423.59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15">
+        <v>421.91</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15">
+        <v>435.41</v>
+      </c>
+      <c r="J15">
+        <v>459.4</v>
+      </c>
+      <c r="M15">
+        <v>426.62</v>
+      </c>
+      <c r="N15">
+        <v>465.09</v>
+      </c>
+      <c r="O15" s="11"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>425.69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16">
+        <v>417.12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="11"/>
+      <c r="I16">
+        <v>437.86</v>
+      </c>
+      <c r="J16">
+        <v>457.5</v>
+      </c>
+      <c r="M16">
+        <v>430.94</v>
+      </c>
+      <c r="N16">
+        <v>456.56</v>
+      </c>
+      <c r="O16" s="11"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <v>414.36</v>
+      </c>
+      <c r="C17" s="44">
+        <v>573.13</v>
+      </c>
+      <c r="F17">
+        <v>425.8</v>
+      </c>
+      <c r="G17" s="44">
+        <v>536.9</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17">
+        <v>430.54</v>
+      </c>
+      <c r="J17">
+        <v>458.23</v>
+      </c>
+      <c r="M17">
+        <v>437.15</v>
+      </c>
+      <c r="N17">
+        <v>458.14</v>
+      </c>
+      <c r="O17" s="11"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="11"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="36"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="11"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="11"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="11"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="11"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="11"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="11"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="11"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="11"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I28" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="39"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
+    </row>
+    <row r="33" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="39"/>
+    </row>
+    <row r="34" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
+    </row>
+    <row r="35" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="I20:N26"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I28:N35"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="I11:N11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2476,39 +3323,39 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2524,10 +3371,10 @@
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="17" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="H3" s="17">
         <f>(8000/1000000000)*1000000</f>
@@ -2561,7 +3408,7 @@
         <v>34</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="H4" s="17">
         <f>(8000/750000000)*1000000</f>
@@ -2595,7 +3442,7 @@
         <v>36</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="H5" s="17">
         <f>(8000/500000000)*1000000</f>
@@ -2629,7 +3476,7 @@
         <v>35</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="H6" s="17">
         <f>(8000/250000000)*1000000</f>
@@ -2657,7 +3504,7 @@
         <v>800000</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="H7" s="17">
         <v>100</v>
@@ -2669,607 +3516,620 @@
       <c r="K7" s="17"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="30" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30" t="s">
+      <c r="E10" s="41"/>
+      <c r="F10" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="30" t="s">
+      <c r="G10" s="41"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30" t="s">
+      <c r="J10" s="41"/>
+      <c r="K10" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30" t="s">
+      <c r="L10" s="41"/>
+      <c r="M10" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="N10" s="30"/>
+      <c r="N10" s="41"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="N11" s="27" t="s">
+      <c r="B11" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="34">
+      <c r="A12" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="28">
         <v>374.85</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C12" s="28">
         <v>415.34</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="28">
         <v>366.98</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="28">
         <v>398.13</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="29">
         <v>387.3</v>
       </c>
-      <c r="G12" s="35">
+      <c r="G12" s="29">
         <v>315.35000000000002</v>
       </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="34">
+      <c r="H12" s="27"/>
+      <c r="I12" s="28">
         <v>384.01</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="28">
         <v>407.92</v>
       </c>
-      <c r="K12" s="34">
+      <c r="K12" s="28">
         <v>386.06</v>
       </c>
-      <c r="L12" s="34">
+      <c r="L12" s="28">
         <v>406.31</v>
       </c>
-      <c r="M12" s="34">
+      <c r="M12" s="28">
         <v>383.38</v>
       </c>
-      <c r="N12" s="34">
+      <c r="N12" s="28">
         <v>406.07</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="34">
+      <c r="A13" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="28">
         <v>381.51</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="28">
         <v>421.74</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="29">
         <v>344.71</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="28">
         <v>399.6</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="28">
         <v>369.4</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="28">
         <v>400.24</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34">
+      <c r="H13" s="27"/>
+      <c r="I13" s="28">
         <v>388.87</v>
       </c>
-      <c r="J13" s="36">
+      <c r="J13" s="30">
         <v>409.9</v>
       </c>
-      <c r="K13" s="34">
+      <c r="K13" s="28">
         <v>392.51</v>
       </c>
-      <c r="L13" s="34">
+      <c r="L13" s="28">
         <v>413.47</v>
       </c>
-      <c r="M13" s="34">
+      <c r="M13" s="28">
         <v>379.55</v>
       </c>
-      <c r="N13" s="34">
+      <c r="N13" s="28">
         <v>395.22</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="28" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="30" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30" t="s">
+      <c r="C17" s="41"/>
+      <c r="D17" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30" t="s">
+      <c r="E17" s="41"/>
+      <c r="F17" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="30" t="s">
+      <c r="G17" s="41"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30" t="s">
+      <c r="J17" s="41"/>
+      <c r="K17" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30" t="s">
+      <c r="L17" s="41"/>
+      <c r="M17" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="N17" s="30"/>
+      <c r="N17" s="41"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="33"/>
-      <c r="I18" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="L18" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="M18" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="N18" s="27" t="s">
+      <c r="A18" s="28"/>
+      <c r="B18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="27"/>
+      <c r="I18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="28">
+        <v>399.19</v>
+      </c>
+      <c r="C19" s="28">
+        <v>419.46</v>
+      </c>
+      <c r="D19" s="28">
+        <v>398.55</v>
+      </c>
+      <c r="E19" s="28">
+        <v>417.53</v>
+      </c>
+      <c r="F19" s="28">
+        <v>406.5</v>
+      </c>
+      <c r="G19" s="28">
+        <v>419.33</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="28">
+        <v>410.13</v>
+      </c>
+      <c r="J19" s="28">
+        <v>432.42</v>
+      </c>
+      <c r="K19" s="28">
+        <v>409.44</v>
+      </c>
+      <c r="L19" s="28">
+        <v>433.99</v>
+      </c>
+      <c r="M19" s="28">
+        <v>417.48</v>
+      </c>
+      <c r="N19" s="28">
+        <v>432.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="28">
+        <v>407.6</v>
+      </c>
+      <c r="C20" s="28">
+        <v>425.83</v>
+      </c>
+      <c r="D20" s="28">
+        <v>403.92</v>
+      </c>
+      <c r="E20" s="28">
+        <v>417.74</v>
+      </c>
+      <c r="F20" s="28">
+        <v>401.51</v>
+      </c>
+      <c r="G20" s="28">
+        <v>416.84</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="28">
+        <v>420.73</v>
+      </c>
+      <c r="J20" s="28">
+        <v>434.88</v>
+      </c>
+      <c r="K20" s="28">
+        <v>417.42</v>
+      </c>
+      <c r="L20" s="28">
+        <v>436.56</v>
+      </c>
+      <c r="M20" s="28">
+        <v>408.77</v>
+      </c>
+      <c r="N20" s="28">
+        <v>431.37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="41"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="27"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="34">
-        <v>399.19</v>
-      </c>
-      <c r="C19" s="34">
-        <v>419.46</v>
-      </c>
-      <c r="D19" s="34">
-        <v>398.55</v>
-      </c>
-      <c r="E19" s="34">
-        <v>417.53</v>
-      </c>
-      <c r="F19" s="34">
-        <v>406.5</v>
-      </c>
-      <c r="G19" s="34">
-        <v>419.33</v>
-      </c>
-      <c r="H19" s="33"/>
-      <c r="I19" s="34">
-        <v>410.13</v>
-      </c>
-      <c r="J19" s="34">
-        <v>432.42</v>
-      </c>
-      <c r="K19" s="34">
-        <v>409.44</v>
-      </c>
-      <c r="L19" s="34">
-        <v>433.99</v>
-      </c>
-      <c r="M19" s="34">
-        <v>417.48</v>
-      </c>
-      <c r="N19" s="34">
-        <v>432.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="B26" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="27"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="34">
-        <v>407.6</v>
-      </c>
-      <c r="C20" s="34">
-        <v>425.83</v>
-      </c>
-      <c r="D20" s="34">
-        <v>403.92</v>
-      </c>
-      <c r="E20" s="34">
-        <v>417.74</v>
-      </c>
-      <c r="F20" s="34">
-        <v>401.51</v>
-      </c>
-      <c r="G20" s="34">
-        <v>416.84</v>
-      </c>
-      <c r="H20" s="33"/>
-      <c r="I20" s="34">
-        <v>420.73</v>
-      </c>
-      <c r="J20" s="34">
-        <v>434.88</v>
-      </c>
-      <c r="K20" s="34">
-        <v>417.42</v>
-      </c>
-      <c r="L20" s="34">
-        <v>436.56</v>
-      </c>
-      <c r="M20" s="34">
-        <v>408.77</v>
-      </c>
-      <c r="N20" s="34">
-        <v>431.37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
-    </row>
-    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
-      <c r="B23" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="30"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="33"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" s="33"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="39"/>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G27" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="39"/>
+      <c r="B27" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="27"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="33"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
+      <c r="B28" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="27"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G29" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="33"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
+      <c r="B29" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="H29" s="27"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="I23:N29"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="I16:N16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="I9:N9"/>
     <mergeCell ref="B10:C10"/>
@@ -3278,26 +4138,13 @@
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="M10:N10"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="I16:N16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="I23:N29"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="R29:AC37"/>
   <sheetViews>
@@ -3308,132 +4155,132 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="29" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R29" s="21" t="s">
+      <c r="R29" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="S29" s="26"/>
-      <c r="T29" s="26"/>
-      <c r="U29" s="26"/>
-      <c r="V29" s="26"/>
-      <c r="W29" s="26"/>
-      <c r="X29" s="26"/>
-      <c r="Y29" s="26"/>
-      <c r="Z29" s="26"/>
-      <c r="AA29" s="26"/>
-      <c r="AB29" s="26"/>
-      <c r="AC29" s="26"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="37"/>
+      <c r="U29" s="37"/>
+      <c r="V29" s="37"/>
+      <c r="W29" s="37"/>
+      <c r="X29" s="37"/>
+      <c r="Y29" s="37"/>
+      <c r="Z29" s="37"/>
+      <c r="AA29" s="37"/>
+      <c r="AB29" s="37"/>
+      <c r="AC29" s="37"/>
     </row>
     <row r="30" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R30" s="26"/>
-      <c r="S30" s="26"/>
-      <c r="T30" s="26"/>
-      <c r="U30" s="26"/>
-      <c r="V30" s="26"/>
-      <c r="W30" s="26"/>
-      <c r="X30" s="26"/>
-      <c r="Y30" s="26"/>
-      <c r="Z30" s="26"/>
-      <c r="AA30" s="26"/>
-      <c r="AB30" s="26"/>
-      <c r="AC30" s="26"/>
+      <c r="R30" s="37"/>
+      <c r="S30" s="37"/>
+      <c r="T30" s="37"/>
+      <c r="U30" s="37"/>
+      <c r="V30" s="37"/>
+      <c r="W30" s="37"/>
+      <c r="X30" s="37"/>
+      <c r="Y30" s="37"/>
+      <c r="Z30" s="37"/>
+      <c r="AA30" s="37"/>
+      <c r="AB30" s="37"/>
+      <c r="AC30" s="37"/>
     </row>
     <row r="31" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R31" s="26"/>
-      <c r="S31" s="26"/>
-      <c r="T31" s="26"/>
-      <c r="U31" s="26"/>
-      <c r="V31" s="26"/>
-      <c r="W31" s="26"/>
-      <c r="X31" s="26"/>
-      <c r="Y31" s="26"/>
-      <c r="Z31" s="26"/>
-      <c r="AA31" s="26"/>
-      <c r="AB31" s="26"/>
-      <c r="AC31" s="26"/>
+      <c r="R31" s="37"/>
+      <c r="S31" s="37"/>
+      <c r="T31" s="37"/>
+      <c r="U31" s="37"/>
+      <c r="V31" s="37"/>
+      <c r="W31" s="37"/>
+      <c r="X31" s="37"/>
+      <c r="Y31" s="37"/>
+      <c r="Z31" s="37"/>
+      <c r="AA31" s="37"/>
+      <c r="AB31" s="37"/>
+      <c r="AC31" s="37"/>
     </row>
     <row r="32" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R32" s="26"/>
-      <c r="S32" s="26"/>
-      <c r="T32" s="26"/>
-      <c r="U32" s="26"/>
-      <c r="V32" s="26"/>
-      <c r="W32" s="26"/>
-      <c r="X32" s="26"/>
-      <c r="Y32" s="26"/>
-      <c r="Z32" s="26"/>
-      <c r="AA32" s="26"/>
-      <c r="AB32" s="26"/>
-      <c r="AC32" s="26"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="37"/>
+      <c r="T32" s="37"/>
+      <c r="U32" s="37"/>
+      <c r="V32" s="37"/>
+      <c r="W32" s="37"/>
+      <c r="X32" s="37"/>
+      <c r="Y32" s="37"/>
+      <c r="Z32" s="37"/>
+      <c r="AA32" s="37"/>
+      <c r="AB32" s="37"/>
+      <c r="AC32" s="37"/>
     </row>
     <row r="33" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R33" s="26"/>
-      <c r="S33" s="26"/>
-      <c r="T33" s="26"/>
-      <c r="U33" s="26"/>
-      <c r="V33" s="26"/>
-      <c r="W33" s="26"/>
-      <c r="X33" s="26"/>
-      <c r="Y33" s="26"/>
-      <c r="Z33" s="26"/>
-      <c r="AA33" s="26"/>
-      <c r="AB33" s="26"/>
-      <c r="AC33" s="26"/>
+      <c r="R33" s="37"/>
+      <c r="S33" s="37"/>
+      <c r="T33" s="37"/>
+      <c r="U33" s="37"/>
+      <c r="V33" s="37"/>
+      <c r="W33" s="37"/>
+      <c r="X33" s="37"/>
+      <c r="Y33" s="37"/>
+      <c r="Z33" s="37"/>
+      <c r="AA33" s="37"/>
+      <c r="AB33" s="37"/>
+      <c r="AC33" s="37"/>
     </row>
     <row r="34" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R34" s="26"/>
-      <c r="S34" s="26"/>
-      <c r="T34" s="26"/>
-      <c r="U34" s="26"/>
-      <c r="V34" s="26"/>
-      <c r="W34" s="26"/>
-      <c r="X34" s="26"/>
-      <c r="Y34" s="26"/>
-      <c r="Z34" s="26"/>
-      <c r="AA34" s="26"/>
-      <c r="AB34" s="26"/>
-      <c r="AC34" s="26"/>
+      <c r="R34" s="37"/>
+      <c r="S34" s="37"/>
+      <c r="T34" s="37"/>
+      <c r="U34" s="37"/>
+      <c r="V34" s="37"/>
+      <c r="W34" s="37"/>
+      <c r="X34" s="37"/>
+      <c r="Y34" s="37"/>
+      <c r="Z34" s="37"/>
+      <c r="AA34" s="37"/>
+      <c r="AB34" s="37"/>
+      <c r="AC34" s="37"/>
     </row>
     <row r="35" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R35" s="26"/>
-      <c r="S35" s="26"/>
-      <c r="T35" s="26"/>
-      <c r="U35" s="26"/>
-      <c r="V35" s="26"/>
-      <c r="W35" s="26"/>
-      <c r="X35" s="26"/>
-      <c r="Y35" s="26"/>
-      <c r="Z35" s="26"/>
-      <c r="AA35" s="26"/>
-      <c r="AB35" s="26"/>
-      <c r="AC35" s="26"/>
+      <c r="R35" s="37"/>
+      <c r="S35" s="37"/>
+      <c r="T35" s="37"/>
+      <c r="U35" s="37"/>
+      <c r="V35" s="37"/>
+      <c r="W35" s="37"/>
+      <c r="X35" s="37"/>
+      <c r="Y35" s="37"/>
+      <c r="Z35" s="37"/>
+      <c r="AA35" s="37"/>
+      <c r="AB35" s="37"/>
+      <c r="AC35" s="37"/>
     </row>
     <row r="36" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R36" s="26"/>
-      <c r="S36" s="26"/>
-      <c r="T36" s="26"/>
-      <c r="U36" s="26"/>
-      <c r="V36" s="26"/>
-      <c r="W36" s="26"/>
-      <c r="X36" s="26"/>
-      <c r="Y36" s="26"/>
-      <c r="Z36" s="26"/>
-      <c r="AA36" s="26"/>
-      <c r="AB36" s="26"/>
-      <c r="AC36" s="26"/>
+      <c r="R36" s="37"/>
+      <c r="S36" s="37"/>
+      <c r="T36" s="37"/>
+      <c r="U36" s="37"/>
+      <c r="V36" s="37"/>
+      <c r="W36" s="37"/>
+      <c r="X36" s="37"/>
+      <c r="Y36" s="37"/>
+      <c r="Z36" s="37"/>
+      <c r="AA36" s="37"/>
+      <c r="AB36" s="37"/>
+      <c r="AC36" s="37"/>
     </row>
     <row r="37" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R37" s="26"/>
-      <c r="S37" s="26"/>
-      <c r="T37" s="26"/>
-      <c r="U37" s="26"/>
-      <c r="V37" s="26"/>
-      <c r="W37" s="26"/>
-      <c r="X37" s="26"/>
-      <c r="Y37" s="26"/>
-      <c r="Z37" s="26"/>
-      <c r="AA37" s="26"/>
-      <c r="AB37" s="26"/>
-      <c r="AC37" s="26"/>
+      <c r="R37" s="37"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="37"/>
+      <c r="U37" s="37"/>
+      <c r="V37" s="37"/>
+      <c r="W37" s="37"/>
+      <c r="X37" s="37"/>
+      <c r="Y37" s="37"/>
+      <c r="Z37" s="37"/>
+      <c r="AA37" s="37"/>
+      <c r="AB37" s="37"/>
+      <c r="AC37" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated some missing low priority values in the iperf at 0.1s sheet
Signed-off-by: Ashish K <akashina@eng.ucsd.edu>
</commit_message>
<xml_diff>
--- a/PriorityExperiments.xlsx
+++ b/PriorityExperiments.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="97">
   <si>
     <t>300k packets @ 100us</t>
   </si>
@@ -565,6 +565,51 @@
   </si>
   <si>
     <t>318 ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.92 ms </t>
+  </si>
+  <si>
+    <t>420 ms</t>
+  </si>
+  <si>
+    <t>387.77ms</t>
+  </si>
+  <si>
+    <t>323.6ms</t>
+  </si>
+  <si>
+    <t>743.5 us</t>
+  </si>
+  <si>
+    <t>573.13 us</t>
+  </si>
+  <si>
+    <t>536.9 us</t>
+  </si>
+  <si>
+    <t>463.96 us</t>
+  </si>
+  <si>
+    <t>459.4 us</t>
+  </si>
+  <si>
+    <t>457.5 us</t>
+  </si>
+  <si>
+    <t>458.23 us</t>
+  </si>
+  <si>
+    <t>454.175 us</t>
+  </si>
+  <si>
+    <t>465.09 us</t>
+  </si>
+  <si>
+    <t>456.56 us</t>
+  </si>
+  <si>
+    <t>458.14 us</t>
   </si>
 </sst>
 </file>
@@ -675,7 +720,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -749,6 +794,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -759,21 +807,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -782,9 +827,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1172,58 +1218,58 @@
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="35"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="3"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="3"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="35"/>
+      <c r="L2" s="36"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="35"/>
+      <c r="P2" s="36"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="6"/>
-      <c r="S2" s="35" t="s">
+      <c r="S2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="35"/>
+      <c r="T2" s="36"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1418,248 +1464,248 @@
       <c r="R7" s="8"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="34"/>
-      <c r="T12" s="34"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="35"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-      <c r="T13" s="34"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="35"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="34"/>
-      <c r="T14" s="34"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="35"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="35"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="34"/>
-      <c r="T16" s="34"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="35"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="34"/>
-      <c r="T17" s="34"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="34"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="35"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="34"/>
-      <c r="S19" s="34"/>
-      <c r="T19" s="34"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
+      <c r="T19" s="35"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="34"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="34"/>
-      <c r="T21" s="34"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
     </row>
     <row r="22" spans="1:20" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="34"/>
-      <c r="T22" s="34"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1703,72 +1749,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36" t="s">
+      <c r="J3" s="39"/>
+      <c r="K3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36" t="s">
+      <c r="L3" s="39"/>
+      <c r="M3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="36"/>
+      <c r="N3" s="39"/>
       <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1949,52 +1995,52 @@
       <c r="O10" s="12"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="35" t="s">
+      <c r="I11" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
       <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36" t="s">
+      <c r="C12" s="39"/>
+      <c r="D12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36" t="s">
+      <c r="E12" s="39"/>
+      <c r="F12" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="36"/>
+      <c r="G12" s="39"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="36" t="s">
+      <c r="I12" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36" t="s">
+      <c r="J12" s="39"/>
+      <c r="K12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36" t="s">
+      <c r="L12" s="39"/>
+      <c r="M12" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="36"/>
+      <c r="N12" s="39"/>
       <c r="O12" s="11"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2172,46 +2218,46 @@
       <c r="O19" s="12"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
       <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36" t="s">
+      <c r="C21" s="39"/>
+      <c r="D21" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36" t="s">
+      <c r="E21" s="39"/>
+      <c r="F21" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="36"/>
+      <c r="G21" s="39"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
       <c r="O21" s="11"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2234,12 +2280,12 @@
         <v>10</v>
       </c>
       <c r="H22" s="11"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
       <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2265,12 +2311,12 @@
         <v>40</v>
       </c>
       <c r="H23" s="11"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
       <c r="O23" s="11"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2296,12 +2342,12 @@
         <v>40</v>
       </c>
       <c r="H24" s="11"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
       <c r="O24" s="11"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2327,12 +2373,12 @@
         <v>40</v>
       </c>
       <c r="H25" s="11"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
       <c r="O25" s="11"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2358,86 +2404,93 @@
         <v>40</v>
       </c>
       <c r="H26" s="11"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="37"/>
-      <c r="N26" s="37"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="40"/>
       <c r="O26" s="11"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I28" s="38" t="s">
+      <c r="I28" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>43</v>
       </c>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
     </row>
     <row r="33" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="39"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
     </row>
     <row r="34" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
     </row>
     <row r="35" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="38"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="23">
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I20:N26"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="I28:N35"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="I3:J3"/>
@@ -2454,13 +2507,6 @@
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I20:N26"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2472,7 +2518,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2491,75 +2537,76 @@
     <col min="13" max="13" width="14.140625" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36" t="s">
+      <c r="J3" s="39"/>
+      <c r="K3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36" t="s">
+      <c r="L3" s="39"/>
+      <c r="M3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="36"/>
+      <c r="N3" s="39"/>
       <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2612,8 +2659,14 @@
       <c r="B5">
         <v>433.25</v>
       </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
       <c r="F5">
         <v>412.95</v>
+      </c>
+      <c r="G5" t="s">
+        <v>84</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5">
@@ -2644,6 +2697,9 @@
       <c r="F6">
         <v>398.71</v>
       </c>
+      <c r="G6" t="s">
+        <v>85</v>
+      </c>
       <c r="H6" s="11"/>
       <c r="I6" s="14">
         <v>430.68</v>
@@ -2672,8 +2728,8 @@
       <c r="F7">
         <v>406.6</v>
       </c>
-      <c r="G7">
-        <v>8.92</v>
+      <c r="G7" t="s">
+        <v>82</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7">
@@ -2710,8 +2766,8 @@
       <c r="I8">
         <v>413.53</v>
       </c>
-      <c r="J8">
-        <v>743.5</v>
+      <c r="J8" t="s">
+        <v>86</v>
       </c>
       <c r="M8">
         <v>419.68</v>
@@ -2756,52 +2812,52 @@
       <c r="O10" s="12"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="35" t="s">
+      <c r="I11" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
       <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36" t="s">
+      <c r="C12" s="39"/>
+      <c r="D12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36" t="s">
+      <c r="E12" s="39"/>
+      <c r="F12" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="36"/>
+      <c r="G12" s="39"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="36" t="s">
+      <c r="I12" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36" t="s">
+      <c r="J12" s="39"/>
+      <c r="K12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36" t="s">
+      <c r="L12" s="39"/>
+      <c r="M12" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="36"/>
+      <c r="N12" s="39"/>
       <c r="O12" s="11"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2864,14 +2920,14 @@
       <c r="I14">
         <v>436.6</v>
       </c>
-      <c r="J14" s="14">
-        <v>463.96</v>
+      <c r="J14" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="M14">
         <v>428.98</v>
       </c>
-      <c r="N14" s="14">
-        <v>454.17500000000001</v>
+      <c r="N14" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="O14" s="11"/>
     </row>
@@ -2882,27 +2938,27 @@
       <c r="B15">
         <v>423.59</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="45" t="s">
         <v>67</v>
       </c>
       <c r="F15">
         <v>421.91</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="45" t="s">
         <v>68</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15">
         <v>435.41</v>
       </c>
-      <c r="J15">
-        <v>459.4</v>
+      <c r="J15" t="s">
+        <v>90</v>
       </c>
       <c r="M15">
         <v>426.62</v>
       </c>
-      <c r="N15">
-        <v>465.09</v>
+      <c r="N15" t="s">
+        <v>94</v>
       </c>
       <c r="O15" s="11"/>
     </row>
@@ -2926,14 +2982,14 @@
       <c r="I16">
         <v>437.86</v>
       </c>
-      <c r="J16">
-        <v>457.5</v>
+      <c r="J16" t="s">
+        <v>91</v>
       </c>
       <c r="M16">
         <v>430.94</v>
       </c>
-      <c r="N16">
-        <v>456.56</v>
+      <c r="N16" t="s">
+        <v>95</v>
       </c>
       <c r="O16" s="11"/>
     </row>
@@ -2944,27 +3000,27 @@
       <c r="B17">
         <v>414.36</v>
       </c>
-      <c r="C17" s="44">
-        <v>573.13</v>
+      <c r="C17" s="33" t="s">
+        <v>87</v>
       </c>
       <c r="F17">
         <v>425.8</v>
       </c>
-      <c r="G17" s="44">
-        <v>536.9</v>
+      <c r="G17" s="33" t="s">
+        <v>88</v>
       </c>
       <c r="H17" s="11"/>
       <c r="I17">
         <v>430.54</v>
       </c>
-      <c r="J17">
-        <v>458.23</v>
+      <c r="J17" t="s">
+        <v>92</v>
       </c>
       <c r="M17">
         <v>437.15</v>
       </c>
-      <c r="N17">
-        <v>458.14</v>
+      <c r="N17" t="s">
+        <v>96</v>
       </c>
       <c r="O17" s="11"/>
     </row>
@@ -3003,46 +3059,46 @@
       <c r="O19" s="12"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
       <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36" t="s">
+      <c r="C21" s="39"/>
+      <c r="D21" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36" t="s">
+      <c r="E21" s="39"/>
+      <c r="F21" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="36"/>
+      <c r="G21" s="39"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
       <c r="O21" s="11"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -3065,12 +3121,12 @@
         <v>10</v>
       </c>
       <c r="H22" s="11"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
       <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -3096,12 +3152,12 @@
         <v>40</v>
       </c>
       <c r="H23" s="11"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
       <c r="O23" s="11"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -3127,12 +3183,12 @@
         <v>40</v>
       </c>
       <c r="H24" s="11"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
       <c r="O24" s="11"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -3158,12 +3214,12 @@
         <v>40</v>
       </c>
       <c r="H25" s="11"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
       <c r="O25" s="11"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -3189,90 +3245,94 @@
         <v>40</v>
       </c>
       <c r="H26" s="11"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="37"/>
-      <c r="N26" s="37"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="40"/>
       <c r="O26" s="11"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I28" s="38" t="s">
+      <c r="I28" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>43</v>
       </c>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
     </row>
     <row r="33" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="39"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
     </row>
     <row r="34" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
     </row>
     <row r="35" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="I20:N26"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="I28:N35"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="I11:N11"/>
@@ -3282,15 +3342,11 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="M12:N12"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="I20:N26"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3301,7 +3357,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12:N12"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3517,51 +3573,51 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
       <c r="H9" s="23"/>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41" t="s">
+      <c r="C10" s="44"/>
+      <c r="D10" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41" t="s">
+      <c r="E10" s="44"/>
+      <c r="F10" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="41"/>
+      <c r="G10" s="44"/>
       <c r="H10" s="25"/>
-      <c r="I10" s="41" t="s">
+      <c r="I10" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41" t="s">
+      <c r="J10" s="44"/>
+      <c r="K10" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41" t="s">
+      <c r="L10" s="44"/>
+      <c r="M10" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="N10" s="41"/>
+      <c r="N10" s="44"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
@@ -3723,51 +3779,51 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="27"/>
-      <c r="I16" s="40" t="s">
+      <c r="I16" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41" t="s">
+      <c r="E17" s="44"/>
+      <c r="F17" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="41"/>
+      <c r="G17" s="44"/>
       <c r="H17" s="27"/>
-      <c r="I17" s="41" t="s">
+      <c r="I17" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41" t="s">
+      <c r="J17" s="44"/>
+      <c r="K17" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41" t="s">
+      <c r="L17" s="44"/>
+      <c r="M17" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="N17" s="41"/>
+      <c r="N17" s="44"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
@@ -3927,14 +3983,14 @@
     </row>
     <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
       <c r="H23" s="27"/>
       <c r="I23" s="42" t="s">
         <v>60</v>
@@ -3947,18 +4003,18 @@
     </row>
     <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41" t="s">
+      <c r="C24" s="44"/>
+      <c r="D24" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41" t="s">
+      <c r="E24" s="44"/>
+      <c r="F24" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="41"/>
+      <c r="G24" s="44"/>
       <c r="H24" s="27"/>
       <c r="I24" s="43"/>
       <c r="J24" s="43"/>
@@ -4117,11 +4173,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="I23:N29"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="I16:N16"/>
     <mergeCell ref="B17:C17"/>
@@ -4130,14 +4189,11 @@
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="K17:L17"/>
     <mergeCell ref="M17:N17"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="I9:N9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="I23:N29"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4155,132 +4211,132 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="29" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R29" s="34" t="s">
+      <c r="R29" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="S29" s="37"/>
-      <c r="T29" s="37"/>
-      <c r="U29" s="37"/>
-      <c r="V29" s="37"/>
-      <c r="W29" s="37"/>
-      <c r="X29" s="37"/>
-      <c r="Y29" s="37"/>
-      <c r="Z29" s="37"/>
-      <c r="AA29" s="37"/>
-      <c r="AB29" s="37"/>
-      <c r="AC29" s="37"/>
+      <c r="S29" s="40"/>
+      <c r="T29" s="40"/>
+      <c r="U29" s="40"/>
+      <c r="V29" s="40"/>
+      <c r="W29" s="40"/>
+      <c r="X29" s="40"/>
+      <c r="Y29" s="40"/>
+      <c r="Z29" s="40"/>
+      <c r="AA29" s="40"/>
+      <c r="AB29" s="40"/>
+      <c r="AC29" s="40"/>
     </row>
     <row r="30" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R30" s="37"/>
-      <c r="S30" s="37"/>
-      <c r="T30" s="37"/>
-      <c r="U30" s="37"/>
-      <c r="V30" s="37"/>
-      <c r="W30" s="37"/>
-      <c r="X30" s="37"/>
-      <c r="Y30" s="37"/>
-      <c r="Z30" s="37"/>
-      <c r="AA30" s="37"/>
-      <c r="AB30" s="37"/>
-      <c r="AC30" s="37"/>
+      <c r="R30" s="40"/>
+      <c r="S30" s="40"/>
+      <c r="T30" s="40"/>
+      <c r="U30" s="40"/>
+      <c r="V30" s="40"/>
+      <c r="W30" s="40"/>
+      <c r="X30" s="40"/>
+      <c r="Y30" s="40"/>
+      <c r="Z30" s="40"/>
+      <c r="AA30" s="40"/>
+      <c r="AB30" s="40"/>
+      <c r="AC30" s="40"/>
     </row>
     <row r="31" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R31" s="37"/>
-      <c r="S31" s="37"/>
-      <c r="T31" s="37"/>
-      <c r="U31" s="37"/>
-      <c r="V31" s="37"/>
-      <c r="W31" s="37"/>
-      <c r="X31" s="37"/>
-      <c r="Y31" s="37"/>
-      <c r="Z31" s="37"/>
-      <c r="AA31" s="37"/>
-      <c r="AB31" s="37"/>
-      <c r="AC31" s="37"/>
+      <c r="R31" s="40"/>
+      <c r="S31" s="40"/>
+      <c r="T31" s="40"/>
+      <c r="U31" s="40"/>
+      <c r="V31" s="40"/>
+      <c r="W31" s="40"/>
+      <c r="X31" s="40"/>
+      <c r="Y31" s="40"/>
+      <c r="Z31" s="40"/>
+      <c r="AA31" s="40"/>
+      <c r="AB31" s="40"/>
+      <c r="AC31" s="40"/>
     </row>
     <row r="32" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R32" s="37"/>
-      <c r="S32" s="37"/>
-      <c r="T32" s="37"/>
-      <c r="U32" s="37"/>
-      <c r="V32" s="37"/>
-      <c r="W32" s="37"/>
-      <c r="X32" s="37"/>
-      <c r="Y32" s="37"/>
-      <c r="Z32" s="37"/>
-      <c r="AA32" s="37"/>
-      <c r="AB32" s="37"/>
-      <c r="AC32" s="37"/>
+      <c r="R32" s="40"/>
+      <c r="S32" s="40"/>
+      <c r="T32" s="40"/>
+      <c r="U32" s="40"/>
+      <c r="V32" s="40"/>
+      <c r="W32" s="40"/>
+      <c r="X32" s="40"/>
+      <c r="Y32" s="40"/>
+      <c r="Z32" s="40"/>
+      <c r="AA32" s="40"/>
+      <c r="AB32" s="40"/>
+      <c r="AC32" s="40"/>
     </row>
     <row r="33" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R33" s="37"/>
-      <c r="S33" s="37"/>
-      <c r="T33" s="37"/>
-      <c r="U33" s="37"/>
-      <c r="V33" s="37"/>
-      <c r="W33" s="37"/>
-      <c r="X33" s="37"/>
-      <c r="Y33" s="37"/>
-      <c r="Z33" s="37"/>
-      <c r="AA33" s="37"/>
-      <c r="AB33" s="37"/>
-      <c r="AC33" s="37"/>
+      <c r="R33" s="40"/>
+      <c r="S33" s="40"/>
+      <c r="T33" s="40"/>
+      <c r="U33" s="40"/>
+      <c r="V33" s="40"/>
+      <c r="W33" s="40"/>
+      <c r="X33" s="40"/>
+      <c r="Y33" s="40"/>
+      <c r="Z33" s="40"/>
+      <c r="AA33" s="40"/>
+      <c r="AB33" s="40"/>
+      <c r="AC33" s="40"/>
     </row>
     <row r="34" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R34" s="37"/>
-      <c r="S34" s="37"/>
-      <c r="T34" s="37"/>
-      <c r="U34" s="37"/>
-      <c r="V34" s="37"/>
-      <c r="W34" s="37"/>
-      <c r="X34" s="37"/>
-      <c r="Y34" s="37"/>
-      <c r="Z34" s="37"/>
-      <c r="AA34" s="37"/>
-      <c r="AB34" s="37"/>
-      <c r="AC34" s="37"/>
+      <c r="R34" s="40"/>
+      <c r="S34" s="40"/>
+      <c r="T34" s="40"/>
+      <c r="U34" s="40"/>
+      <c r="V34" s="40"/>
+      <c r="W34" s="40"/>
+      <c r="X34" s="40"/>
+      <c r="Y34" s="40"/>
+      <c r="Z34" s="40"/>
+      <c r="AA34" s="40"/>
+      <c r="AB34" s="40"/>
+      <c r="AC34" s="40"/>
     </row>
     <row r="35" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R35" s="37"/>
-      <c r="S35" s="37"/>
-      <c r="T35" s="37"/>
-      <c r="U35" s="37"/>
-      <c r="V35" s="37"/>
-      <c r="W35" s="37"/>
-      <c r="X35" s="37"/>
-      <c r="Y35" s="37"/>
-      <c r="Z35" s="37"/>
-      <c r="AA35" s="37"/>
-      <c r="AB35" s="37"/>
-      <c r="AC35" s="37"/>
+      <c r="R35" s="40"/>
+      <c r="S35" s="40"/>
+      <c r="T35" s="40"/>
+      <c r="U35" s="40"/>
+      <c r="V35" s="40"/>
+      <c r="W35" s="40"/>
+      <c r="X35" s="40"/>
+      <c r="Y35" s="40"/>
+      <c r="Z35" s="40"/>
+      <c r="AA35" s="40"/>
+      <c r="AB35" s="40"/>
+      <c r="AC35" s="40"/>
     </row>
     <row r="36" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R36" s="37"/>
-      <c r="S36" s="37"/>
-      <c r="T36" s="37"/>
-      <c r="U36" s="37"/>
-      <c r="V36" s="37"/>
-      <c r="W36" s="37"/>
-      <c r="X36" s="37"/>
-      <c r="Y36" s="37"/>
-      <c r="Z36" s="37"/>
-      <c r="AA36" s="37"/>
-      <c r="AB36" s="37"/>
-      <c r="AC36" s="37"/>
+      <c r="R36" s="40"/>
+      <c r="S36" s="40"/>
+      <c r="T36" s="40"/>
+      <c r="U36" s="40"/>
+      <c r="V36" s="40"/>
+      <c r="W36" s="40"/>
+      <c r="X36" s="40"/>
+      <c r="Y36" s="40"/>
+      <c r="Z36" s="40"/>
+      <c r="AA36" s="40"/>
+      <c r="AB36" s="40"/>
+      <c r="AC36" s="40"/>
     </row>
     <row r="37" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R37" s="37"/>
-      <c r="S37" s="37"/>
-      <c r="T37" s="37"/>
-      <c r="U37" s="37"/>
-      <c r="V37" s="37"/>
-      <c r="W37" s="37"/>
-      <c r="X37" s="37"/>
-      <c r="Y37" s="37"/>
-      <c r="Z37" s="37"/>
-      <c r="AA37" s="37"/>
-      <c r="AB37" s="37"/>
-      <c r="AC37" s="37"/>
+      <c r="R37" s="40"/>
+      <c r="S37" s="40"/>
+      <c r="T37" s="40"/>
+      <c r="U37" s="40"/>
+      <c r="V37" s="40"/>
+      <c r="W37" s="40"/>
+      <c r="X37" s="40"/>
+      <c r="Y37" s="40"/>
+      <c r="Z37" s="40"/>
+      <c r="AA37" s="40"/>
+      <c r="AB37" s="40"/>
+      <c r="AC37" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>